<commit_message>
added ai search mode using a rag pipeline
</commit_message>
<xml_diff>
--- a/ranked_players.xlsx
+++ b/ranked_players.xlsx
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>7.098891572233441</v>
+        <v>7.09889157223344</v>
       </c>
     </row>
     <row r="4">
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6.233828934358403</v>
+        <v>6.233828934358401</v>
       </c>
     </row>
     <row r="6">
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>6.086936174389221</v>
+        <v>6.086936174389224</v>
       </c>
     </row>
     <row r="10">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>5.924576647265784</v>
+        <v>5.924576647265786</v>
       </c>
     </row>
     <row r="13">
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5.565913387454899</v>
+        <v>5.5659133874549</v>
       </c>
     </row>
     <row r="19">
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5.555754604518879</v>
+        <v>5.555754604518878</v>
       </c>
     </row>
     <row r="21">
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>5.512989783788605</v>
+        <v>5.512989783788603</v>
       </c>
     </row>
     <row r="22">
@@ -733,7 +733,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>5.472145385325657</v>
+        <v>5.472145385325656</v>
       </c>
     </row>
     <row r="24">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.364525752812463</v>
+        <v>5.364525752812462</v>
       </c>
     </row>
     <row r="27">
@@ -798,7 +798,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>5.328173683928732</v>
+        <v>5.328173683928733</v>
       </c>
     </row>
     <row r="29">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5.292544069035512</v>
+        <v>5.292544069035513</v>
       </c>
     </row>
     <row r="33">
@@ -863,7 +863,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>5.280883572062889</v>
+        <v>5.280883572062888</v>
       </c>
     </row>
     <row r="34">
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>5.261378985256923</v>
+        <v>5.261378985256924</v>
       </c>
     </row>
     <row r="35">
@@ -889,7 +889,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>5.193375032878276</v>
+        <v>5.193375032878277</v>
       </c>
     </row>
     <row r="36">
@@ -928,7 +928,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>5.135244912350528</v>
+        <v>5.135244912350529</v>
       </c>
     </row>
     <row r="39">
@@ -993,7 +993,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>5.066888854035263</v>
+        <v>5.066888854035262</v>
       </c>
     </row>
     <row r="44">
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.927732000453152</v>
+        <v>4.927732000453153</v>
       </c>
     </row>
     <row r="52">
@@ -1240,7 +1240,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>4.70395001755988</v>
+        <v>4.703950017559879</v>
       </c>
     </row>
     <row r="63">
@@ -1266,7 +1266,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>4.657264936249884</v>
+        <v>4.657264936249885</v>
       </c>
     </row>
     <row r="65">
@@ -1318,7 +1318,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4.615286112451729</v>
+        <v>4.61528611245173</v>
       </c>
     </row>
     <row r="69">
@@ -1383,7 +1383,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>4.537648866887325</v>
+        <v>4.537648866887326</v>
       </c>
     </row>
     <row r="74">
@@ -1396,7 +1396,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>4.529148693164232</v>
+        <v>4.529148693164231</v>
       </c>
     </row>
     <row r="75">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>4.470301425525825</v>
+        <v>4.470301425525826</v>
       </c>
     </row>
     <row r="77">
@@ -1474,7 +1474,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>4.437626409099299</v>
+        <v>4.437626409099298</v>
       </c>
     </row>
     <row r="81">
@@ -1487,7 +1487,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>4.437120034208006</v>
+        <v>4.437120034208007</v>
       </c>
     </row>
     <row r="82">
@@ -1500,7 +1500,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>4.434103685646993</v>
+        <v>4.434103685646992</v>
       </c>
     </row>
     <row r="83">
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>4.394179713533773</v>
+        <v>4.394179713533774</v>
       </c>
     </row>
     <row r="87">
@@ -1565,7 +1565,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>4.363901975692978</v>
+        <v>4.363901975692979</v>
       </c>
     </row>
     <row r="88">
@@ -1578,7 +1578,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>4.349800716552077</v>
+        <v>4.349800716552076</v>
       </c>
     </row>
     <row r="89">
@@ -1643,7 +1643,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4.257613452816482</v>
+        <v>4.257613452816483</v>
       </c>
     </row>
     <row r="94">
@@ -1721,7 +1721,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>4.136890546629922</v>
+        <v>4.136890546629921</v>
       </c>
     </row>
     <row r="100">
@@ -1734,7 +1734,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>4.132411030482517</v>
+        <v>4.132411030482515</v>
       </c>
     </row>
     <row r="101">
@@ -1838,7 +1838,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>4.09056256161237</v>
+        <v>4.090562561612369</v>
       </c>
     </row>
     <row r="109">
@@ -1851,7 +1851,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>4.08520574231582</v>
+        <v>4.085205742315821</v>
       </c>
     </row>
     <row r="110">
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>4.051447473075985</v>
+        <v>4.051447473075984</v>
       </c>
     </row>
     <row r="113">
@@ -1955,7 +1955,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>4.026692428408428</v>
+        <v>4.026692428408427</v>
       </c>
     </row>
     <row r="118">
@@ -2007,7 +2007,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>3.965904764917341</v>
+        <v>3.965904764917342</v>
       </c>
     </row>
     <row r="122">
@@ -2033,7 +2033,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>3.959750756143302</v>
+        <v>3.959750756143303</v>
       </c>
     </row>
     <row r="124">
@@ -2163,7 +2163,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>3.824648527142564</v>
+        <v>3.824648527142565</v>
       </c>
     </row>
     <row r="134">
@@ -2241,7 +2241,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>3.790377441404375</v>
+        <v>3.790377441404376</v>
       </c>
     </row>
     <row r="140">
@@ -2306,7 +2306,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>3.751595650233416</v>
+        <v>3.751595650233417</v>
       </c>
     </row>
     <row r="145">
@@ -2644,7 +2644,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>3.537061816251393</v>
+        <v>3.537061816251392</v>
       </c>
     </row>
     <row r="171">
@@ -2683,7 +2683,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>3.521481451254267</v>
+        <v>3.521481451254268</v>
       </c>
     </row>
     <row r="174">
@@ -2735,7 +2735,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>3.495326001989773</v>
+        <v>3.495326001989772</v>
       </c>
     </row>
     <row r="178">
@@ -2787,7 +2787,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>3.478474161226249</v>
+        <v>3.478474161226248</v>
       </c>
     </row>
     <row r="182">
@@ -2813,7 +2813,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>3.473579242001733</v>
+        <v>3.473579242001734</v>
       </c>
     </row>
     <row r="184">
@@ -2878,7 +2878,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>3.430304683381625</v>
+        <v>3.430304683381626</v>
       </c>
     </row>
     <row r="189">
@@ -2891,7 +2891,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>3.42886728819851</v>
+        <v>3.428867288198511</v>
       </c>
     </row>
     <row r="190">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>3.375649426719543</v>
+        <v>3.375649426719542</v>
       </c>
     </row>
     <row r="197">
@@ -2995,7 +2995,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>3.375156798440196</v>
+        <v>3.375156798440197</v>
       </c>
     </row>
     <row r="198">
@@ -3190,7 +3190,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>3.307577594561247</v>
+        <v>3.307577594561246</v>
       </c>
     </row>
     <row r="213">
@@ -3242,7 +3242,7 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>3.27618874621971</v>
+        <v>3.276188746219709</v>
       </c>
     </row>
     <row r="217">
@@ -3268,7 +3268,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>3.269608731840827</v>
+        <v>3.269608731840828</v>
       </c>
     </row>
     <row r="219">
@@ -3346,7 +3346,7 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>3.244225082554392</v>
+        <v>3.244225082554393</v>
       </c>
     </row>
     <row r="225">
@@ -3359,7 +3359,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>3.241668429315885</v>
+        <v>3.241668429315886</v>
       </c>
     </row>
     <row r="226">
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>3.230416453223056</v>
+        <v>3.230416453223055</v>
       </c>
     </row>
     <row r="227">
@@ -3541,7 +3541,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>3.143244547684342</v>
+        <v>3.143244547684341</v>
       </c>
     </row>
     <row r="240">
@@ -3554,7 +3554,7 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>3.143095047632652</v>
+        <v>3.143095047632653</v>
       </c>
     </row>
     <row r="241">
@@ -3580,7 +3580,7 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>3.136404394335193</v>
+        <v>3.136404394335194</v>
       </c>
     </row>
     <row r="243">
@@ -3606,7 +3606,7 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>3.132674604859595</v>
+        <v>3.132674604859594</v>
       </c>
     </row>
     <row r="245">
@@ -3632,7 +3632,7 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>3.130575079121082</v>
+        <v>3.130575079121081</v>
       </c>
     </row>
     <row r="247">
@@ -3736,7 +3736,7 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>3.062717522274882</v>
+        <v>3.062717522274881</v>
       </c>
     </row>
     <row r="255">
@@ -3775,7 +3775,7 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>3.049167346726346</v>
+        <v>3.049167346726347</v>
       </c>
     </row>
     <row r="258">
@@ -3788,7 +3788,7 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>3.042466654888294</v>
+        <v>3.042466654888295</v>
       </c>
     </row>
     <row r="259">
@@ -3840,7 +3840,7 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>3.025091235132621</v>
+        <v>3.02509123513262</v>
       </c>
     </row>
     <row r="263">
@@ -3918,7 +3918,7 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>2.992562848145012</v>
+        <v>2.992562848145013</v>
       </c>
     </row>
     <row r="269">
@@ -4165,7 +4165,7 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>2.929075426543308</v>
+        <v>2.929075426543307</v>
       </c>
     </row>
     <row r="288">
@@ -4178,7 +4178,7 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>2.911167232483647</v>
+        <v>2.911167232483646</v>
       </c>
     </row>
     <row r="289">
@@ -4204,7 +4204,7 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>2.907068596781412</v>
+        <v>2.907068596781413</v>
       </c>
     </row>
     <row r="291">
@@ -4308,7 +4308,7 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>2.876954875920991</v>
+        <v>2.876954875920992</v>
       </c>
     </row>
     <row r="299">
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>2.853443551425071</v>
+        <v>2.853443551425072</v>
       </c>
     </row>
     <row r="302">
@@ -4399,7 +4399,7 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>2.819153708928569</v>
+        <v>2.819153708928568</v>
       </c>
     </row>
     <row r="306">
@@ -4451,7 +4451,7 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>2.803368766591179</v>
+        <v>2.803368766591178</v>
       </c>
     </row>
     <row r="310">
@@ -4490,7 +4490,7 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>2.789509185934272</v>
+        <v>2.789509185934271</v>
       </c>
     </row>
     <row r="313">
@@ -4542,7 +4542,7 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>2.743630053180145</v>
+        <v>2.743630053180144</v>
       </c>
     </row>
     <row r="317">
@@ -4620,7 +4620,7 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>2.710056414008831</v>
+        <v>2.710056414008832</v>
       </c>
     </row>
     <row r="323">
@@ -4685,7 +4685,7 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>2.677614335367275</v>
+        <v>2.677614335367276</v>
       </c>
     </row>
     <row r="328">
@@ -4711,7 +4711,7 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>2.671594442854135</v>
+        <v>2.671594442854136</v>
       </c>
     </row>
     <row r="330">
@@ -4815,7 +4815,7 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>2.64013708993979</v>
+        <v>2.640137089939791</v>
       </c>
     </row>
     <row r="338">
@@ -4841,7 +4841,7 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>2.633891661560952</v>
+        <v>2.633891661560951</v>
       </c>
     </row>
     <row r="340">
@@ -4932,7 +4932,7 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>2.581776566828945</v>
+        <v>2.581776566828946</v>
       </c>
     </row>
     <row r="347">
@@ -5010,7 +5010,7 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>2.551121674028084</v>
+        <v>2.551121674028085</v>
       </c>
     </row>
     <row r="353">
@@ -5075,7 +5075,7 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>2.515551552441792</v>
+        <v>2.515551552441791</v>
       </c>
     </row>
     <row r="358">
@@ -5127,7 +5127,7 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>2.488566825694708</v>
+        <v>2.488566825694707</v>
       </c>
     </row>
     <row r="362">
@@ -5257,7 +5257,7 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>2.435501533868815</v>
+        <v>2.435501533868814</v>
       </c>
     </row>
     <row r="372">
@@ -5348,7 +5348,7 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>2.410360759783751</v>
+        <v>2.410360759783752</v>
       </c>
     </row>
     <row r="379">
@@ -5387,7 +5387,7 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>2.405557732068736</v>
+        <v>2.405557732068735</v>
       </c>
     </row>
     <row r="382">
@@ -5491,7 +5491,7 @@
         </is>
       </c>
       <c r="C389" t="n">
-        <v>2.323599091256791</v>
+        <v>2.32359909125679</v>
       </c>
     </row>
     <row r="390">
@@ -5595,7 +5595,7 @@
         </is>
       </c>
       <c r="C397" t="n">
-        <v>2.288388009092275</v>
+        <v>2.288388009092274</v>
       </c>
     </row>
     <row r="398">
@@ -5608,7 +5608,7 @@
         </is>
       </c>
       <c r="C398" t="n">
-        <v>2.287480869997957</v>
+        <v>2.287480869997958</v>
       </c>
     </row>
     <row r="399">
@@ -5634,7 +5634,7 @@
         </is>
       </c>
       <c r="C400" t="n">
-        <v>2.281384883643497</v>
+        <v>2.281384883643496</v>
       </c>
     </row>
     <row r="401">
@@ -5816,7 +5816,7 @@
         </is>
       </c>
       <c r="C414" t="n">
-        <v>2.219961658654752</v>
+        <v>2.219961658654751</v>
       </c>
     </row>
     <row r="415">
@@ -5868,7 +5868,7 @@
         </is>
       </c>
       <c r="C418" t="n">
-        <v>2.205110054963555</v>
+        <v>2.205110054963554</v>
       </c>
     </row>
     <row r="419">
@@ -5881,7 +5881,7 @@
         </is>
       </c>
       <c r="C419" t="n">
-        <v>2.196871436300688</v>
+        <v>2.196871436300689</v>
       </c>
     </row>
     <row r="420">
@@ -5985,7 +5985,7 @@
         </is>
       </c>
       <c r="C427" t="n">
-        <v>2.169571475777011</v>
+        <v>2.16957147577701</v>
       </c>
     </row>
     <row r="428">
@@ -6115,7 +6115,7 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>2.099612930460642</v>
+        <v>2.099612930460641</v>
       </c>
     </row>
     <row r="438">
@@ -6323,7 +6323,7 @@
         </is>
       </c>
       <c r="C453" t="n">
-        <v>1.993584976709155</v>
+        <v>1.993584976709154</v>
       </c>
     </row>
     <row r="454">
@@ -6362,7 +6362,7 @@
         </is>
       </c>
       <c r="C456" t="n">
-        <v>1.991359033064004</v>
+        <v>1.991359033064005</v>
       </c>
     </row>
     <row r="457">
@@ -6440,7 +6440,7 @@
         </is>
       </c>
       <c r="C462" t="n">
-        <v>1.950290425806724</v>
+        <v>1.950290425806723</v>
       </c>
     </row>
     <row r="463">
@@ -6583,7 +6583,7 @@
         </is>
       </c>
       <c r="C473" t="n">
-        <v>1.890642317658675</v>
+        <v>1.890642317658674</v>
       </c>
     </row>
     <row r="474">
@@ -6648,7 +6648,7 @@
         </is>
       </c>
       <c r="C478" t="n">
-        <v>1.868333032424453</v>
+        <v>1.868333032424452</v>
       </c>
     </row>
     <row r="479">
@@ -6739,7 +6739,7 @@
         </is>
       </c>
       <c r="C485" t="n">
-        <v>1.836264244019883</v>
+        <v>1.836264244019882</v>
       </c>
     </row>
     <row r="486">
@@ -6843,7 +6843,7 @@
         </is>
       </c>
       <c r="C493" t="n">
-        <v>1.773123455160446</v>
+        <v>1.773123455160445</v>
       </c>
     </row>
     <row r="494">
@@ -6882,7 +6882,7 @@
         </is>
       </c>
       <c r="C496" t="n">
-        <v>1.746363882895319</v>
+        <v>1.746363882895318</v>
       </c>
     </row>
     <row r="497">
@@ -6934,7 +6934,7 @@
         </is>
       </c>
       <c r="C500" t="n">
-        <v>1.719440480946725</v>
+        <v>1.719440480946724</v>
       </c>
     </row>
     <row r="501">
@@ -6973,7 +6973,7 @@
         </is>
       </c>
       <c r="C503" t="n">
-        <v>1.671124439900589</v>
+        <v>1.671124439900588</v>
       </c>
     </row>
     <row r="504">
@@ -7064,7 +7064,7 @@
         </is>
       </c>
       <c r="C510" t="n">
-        <v>1.627965956698352</v>
+        <v>1.627965956698351</v>
       </c>
     </row>
     <row r="511">
@@ -7155,7 +7155,7 @@
         </is>
       </c>
       <c r="C517" t="n">
-        <v>1.52387726951777</v>
+        <v>1.523877269517771</v>
       </c>
     </row>
     <row r="518">
@@ -7324,7 +7324,7 @@
         </is>
       </c>
       <c r="C530" t="n">
-        <v>1.425171571036262</v>
+        <v>1.425171571036261</v>
       </c>
     </row>
     <row r="531">
@@ -7337,7 +7337,7 @@
         </is>
       </c>
       <c r="C531" t="n">
-        <v>1.398987820671151</v>
+        <v>1.398987820671152</v>
       </c>
     </row>
     <row r="532">
@@ -7480,7 +7480,7 @@
         </is>
       </c>
       <c r="C542" t="n">
-        <v>1.276147349447841</v>
+        <v>1.27614734944784</v>
       </c>
     </row>
     <row r="543">
@@ -7493,7 +7493,7 @@
         </is>
       </c>
       <c r="C543" t="n">
-        <v>1.272850633407213</v>
+        <v>1.272850633407212</v>
       </c>
     </row>
     <row r="544">
@@ -7584,7 +7584,7 @@
         </is>
       </c>
       <c r="C550" t="n">
-        <v>1.180322467804963</v>
+        <v>1.180322467804964</v>
       </c>
     </row>
     <row r="551">
@@ -7753,7 +7753,7 @@
         </is>
       </c>
       <c r="C563" t="n">
-        <v>0.6468563148920177</v>
+        <v>0.6468563148920176</v>
       </c>
     </row>
     <row r="564">

</xml_diff>